<commit_message>
added ndcg & similarity processing
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -14,32 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="22">
-  <si>
-    <t>f5a40228283e40c8a9b1602fe05d3606</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
+  <si>
+    <t>d1373849146249d9ba3d469c9f7bd508</t>
   </si>
   <si>
     <t>ML-Searchengine</t>
   </si>
   <si>
+    <t>Avg. TF-IDF</t>
+  </si>
+  <si>
+    <t>Top TF-IDF</t>
+  </si>
+  <si>
+    <t>nDCG</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
     <t>Fulltext-Searchengine</t>
   </si>
   <si>
-    <t>Avg. TF-IDF</t>
-  </si>
-  <si>
-    <t>Top TF-IDF</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>Recall</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
     <t>Query 1</t>
   </si>
   <si>
@@ -73,13 +70,10 @@
     <t>MAP</t>
   </si>
   <si>
-    <t>beab50d10d0848ba9b2944bf9dbbb1e9</t>
-  </si>
-  <si>
-    <t>1ab066d8adfc41c5838e7ebc908a5765</t>
-  </si>
-  <si>
-    <t>aff48ef9b479476a880f1b2aa9069132</t>
+    <t>c9fd5cda55ed488db73dbb75806f5810</t>
+  </si>
+  <si>
+    <t>d1e07f414cff4a038271f43b379873b6</t>
   </si>
 </sst>
 </file>
@@ -425,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -454,7 +448,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -463,39 +457,33 @@
     </row>
     <row r="3" spans="1:11">
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
       <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>55.39</v>
@@ -504,12 +492,15 @@
         <v>60.9176157115223</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.8491130822519277</v>
+      </c>
+      <c r="E4">
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>76.75</v>
@@ -518,7 +509,10 @@
         <v>87.23094749123473</v>
       </c>
       <c r="D5">
-        <v>0.7</v>
+        <v>0.8201741356762529</v>
+      </c>
+      <c r="E5">
+        <v>0.8</v>
       </c>
       <c r="G5">
         <v>22.66</v>
@@ -527,12 +521,15 @@
         <v>44.04453234215361</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>102.3</v>
@@ -541,6 +538,9 @@
         <v>102.3007008435684</v>
       </c>
       <c r="D6">
+        <v>0.9429942892150167</v>
+      </c>
+      <c r="E6">
         <v>0.8</v>
       </c>
       <c r="G6">
@@ -550,12 +550,15 @@
         <v>53.76228157544278</v>
       </c>
       <c r="I6">
-        <v>0.6</v>
+        <v>0.8631997506525686</v>
+      </c>
+      <c r="J6">
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>38.77</v>
@@ -564,48 +567,56 @@
         <v>38.76666340151514</v>
       </c>
       <c r="D7">
+        <v>0.9469024295259745</v>
+      </c>
+      <c r="E7">
         <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>0.7330126842403628</v>
-      </c>
-      <c r="G13">
-        <v>0.7777248677248676</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>0.7877108134920635</v>
+      </c>
+      <c r="G14">
+        <v>0.8630456349206349</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -626,7 +637,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -635,39 +646,33 @@
     </row>
     <row r="17" spans="1:11">
       <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
       <c r="G17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
         <v>3</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>4</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>5</v>
-      </c>
-      <c r="J17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>55.39</v>
@@ -676,12 +681,15 @@
         <v>60.9176157115223</v>
       </c>
       <c r="D18">
-        <v>0.6</v>
+        <v>0.8631997506525686</v>
+      </c>
+      <c r="E18">
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>76.75</v>
@@ -690,7 +698,10 @@
         <v>87.23094749123473</v>
       </c>
       <c r="D19">
-        <v>0.8</v>
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
       </c>
       <c r="G19">
         <v>22.66</v>
@@ -699,12 +710,15 @@
         <v>44.04453234215361</v>
       </c>
       <c r="I19">
-        <v>0.8</v>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>102.3</v>
@@ -713,6 +727,9 @@
         <v>102.3007008435684</v>
       </c>
       <c r="D20">
+        <v>0.9963488021549354</v>
+      </c>
+      <c r="E20">
         <v>0.8</v>
       </c>
       <c r="G20">
@@ -722,12 +739,15 @@
         <v>53.76228157544278</v>
       </c>
       <c r="I20">
-        <v>0.8</v>
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>38.77</v>
@@ -736,48 +756,56 @@
         <v>38.76666340151514</v>
       </c>
       <c r="D21">
-        <v>0.8</v>
+        <v>0.8529278650606567</v>
+      </c>
+      <c r="E21">
+        <v>0.6</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27">
-        <v>0.7917906746031746</v>
-      </c>
-      <c r="G27">
-        <v>0.8671130952380952</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>0.8530505952380953</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -798,7 +826,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -807,320 +835,285 @@
     </row>
     <row r="31" spans="1:11">
       <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
         <v>3</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>4</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" t="s">
-        <v>7</v>
-      </c>
       <c r="G31" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" t="s">
         <v>3</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>4</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>5</v>
-      </c>
-      <c r="J31" t="s">
-        <v>6</v>
-      </c>
-      <c r="K31" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32">
-        <v>55.39</v>
+        <v>57.02</v>
       </c>
       <c r="C32">
         <v>60.9176157115223</v>
       </c>
       <c r="D32">
+        <v>0.8878428156094799</v>
+      </c>
+      <c r="E32">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>108.55</v>
+      </c>
+      <c r="C33">
+        <v>125.6668670312026</v>
+      </c>
+      <c r="D33">
+        <v>0.6027819274910589</v>
+      </c>
+      <c r="E33">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" t="s">
+      <c r="G33">
+        <v>62.95</v>
+      </c>
+      <c r="H33">
+        <v>70.67666514846523</v>
+      </c>
+      <c r="I33">
+        <v>0.844330763384584</v>
+      </c>
+      <c r="J33">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
         <v>9</v>
       </c>
-      <c r="B33">
-        <v>76.75</v>
-      </c>
-      <c r="C33">
+      <c r="B34">
+        <v>115.41</v>
+      </c>
+      <c r="C34">
+        <v>120.5120388037047</v>
+      </c>
+      <c r="D34">
+        <v>0.7344355650194593</v>
+      </c>
+      <c r="E34">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>52.38</v>
+      </c>
+      <c r="C35">
+        <v>54.85648604463321</v>
+      </c>
+      <c r="D35">
+        <v>0.8401381804368546</v>
+      </c>
+      <c r="E35">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>182.69</v>
+      </c>
+      <c r="C36">
+        <v>184.0350564107108</v>
+      </c>
+      <c r="D36">
+        <v>0.9249372331423046</v>
+      </c>
+      <c r="E36">
+        <v>0.8</v>
+      </c>
+      <c r="G36">
+        <v>126.22</v>
+      </c>
+      <c r="H36">
+        <v>137.4441967422446</v>
+      </c>
+      <c r="I36">
+        <v>0.9670943502702473</v>
+      </c>
+      <c r="J36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>56.81</v>
+      </c>
+      <c r="C37">
+        <v>80.43183878138937</v>
+      </c>
+      <c r="D37">
+        <v>0.8807440226933967</v>
+      </c>
+      <c r="E37">
+        <v>0.6</v>
+      </c>
+      <c r="G37">
+        <v>46.38</v>
+      </c>
+      <c r="H37">
+        <v>62.50397729687458</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <v>131.26</v>
+      </c>
+      <c r="C38">
+        <v>140.0842590305578</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>112.68</v>
+      </c>
+      <c r="H38">
+        <v>118.0223505098338</v>
+      </c>
+      <c r="I38">
+        <v>0.5997437692430793</v>
+      </c>
+      <c r="J38">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>77.25</v>
+      </c>
+      <c r="C39">
         <v>87.23094749123473</v>
       </c>
-      <c r="D33">
+      <c r="D39">
+        <v>0.9384745935215791</v>
+      </c>
+      <c r="E39">
         <v>0.8</v>
       </c>
-      <c r="G33">
+      <c r="G39">
         <v>22.66</v>
       </c>
-      <c r="H33">
+      <c r="H39">
         <v>44.04453234215361</v>
       </c>
-      <c r="I33">
+      <c r="I39">
+        <v>0.9799214801447084</v>
+      </c>
+      <c r="J39">
         <v>0.7</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34">
-        <v>102.3</v>
-      </c>
-      <c r="C34">
-        <v>102.3007008435684</v>
-      </c>
-      <c r="D34">
-        <v>0.7</v>
-      </c>
-      <c r="G34">
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>103.17</v>
+      </c>
+      <c r="C40">
+        <v>103.1696444156127</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="G40">
         <v>53.76</v>
       </c>
-      <c r="H34">
+      <c r="H40">
         <v>53.76228157544278</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35">
+      <c r="I40">
+        <v>0.8165229378311882</v>
+      </c>
+      <c r="J40">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41">
         <v>38.77</v>
       </c>
-      <c r="C35">
+      <c r="C41">
         <v>38.76666340151514</v>
       </c>
-      <c r="D35">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41">
-        <v>0.6910218253968254</v>
-      </c>
-      <c r="G41">
-        <v>0.4194444444444445</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="B43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="B44" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" t="s">
-        <v>3</v>
-      </c>
-      <c r="H45" t="s">
-        <v>4</v>
-      </c>
-      <c r="I45" t="s">
-        <v>5</v>
-      </c>
-      <c r="J45" t="s">
-        <v>6</v>
-      </c>
-      <c r="K45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46">
-        <v>55.39</v>
-      </c>
-      <c r="C46">
-        <v>60.9176157115223</v>
-      </c>
-      <c r="D46">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47">
-        <v>76.75</v>
-      </c>
-      <c r="C47">
-        <v>87.23094749123473</v>
-      </c>
-      <c r="D47">
+      <c r="D41">
+        <v>0.7606395682357036</v>
+      </c>
+      <c r="E41">
         <v>0.8</v>
       </c>
-      <c r="G47">
-        <v>22.66</v>
-      </c>
-      <c r="H47">
-        <v>44.04453234215361</v>
-      </c>
-      <c r="I47">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48">
-        <v>102.3</v>
-      </c>
-      <c r="C48">
-        <v>102.3007008435684</v>
-      </c>
-      <c r="D48">
-        <v>0.9</v>
-      </c>
-      <c r="G48">
-        <v>53.76</v>
-      </c>
-      <c r="H48">
-        <v>53.76228157544278</v>
-      </c>
-      <c r="I48">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49">
-        <v>38.77</v>
-      </c>
-      <c r="C49">
-        <v>38.76666340151514</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55">
-        <v>0.8998980379188712</v>
-      </c>
-      <c r="G55">
-        <v>0.7911493764172335</v>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>0.7463709372637946</v>
+      </c>
+      <c r="G42">
+        <v>0.7814043209876543</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="9">
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:K2"/>
@@ -1130,9 +1123,6 @@
     <mergeCell ref="B29:K29"/>
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="G30:K30"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="G44:K44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated plots for all 10 surveys
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="52">
   <si>
     <t>Avg. TF-IDF</t>
   </si>
@@ -152,6 +152,24 @@
   </si>
   <si>
     <t>0.80</t>
+  </si>
+  <si>
+    <t>User 9</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>User 10</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.48</t>
   </si>
 </sst>
 </file>
@@ -494,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G303"/>
+  <dimension ref="A1:G379"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6711,8 +6729,1560 @@
         <v>26</v>
       </c>
     </row>
+    <row r="305" spans="1:7">
+      <c r="B305" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C305" s="1"/>
+      <c r="D305" s="1"/>
+      <c r="E305" s="1"/>
+      <c r="F305" s="1"/>
+      <c r="G305" s="1"/>
+    </row>
+    <row r="306" spans="1:7">
+      <c r="B306" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C306" s="1"/>
+      <c r="D306" s="1"/>
+      <c r="E306" s="1"/>
+      <c r="F306" s="1"/>
+      <c r="G306" s="1"/>
+    </row>
+    <row r="307" spans="1:7">
+      <c r="B307" t="s">
+        <v>0</v>
+      </c>
+      <c r="C307" t="s">
+        <v>1</v>
+      </c>
+      <c r="D307" t="s">
+        <v>2</v>
+      </c>
+      <c r="E307" t="s">
+        <v>3</v>
+      </c>
+      <c r="F307" t="s">
+        <v>4</v>
+      </c>
+      <c r="G307" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7">
+      <c r="A308" t="s">
+        <v>8</v>
+      </c>
+      <c r="B308">
+        <v>114.36</v>
+      </c>
+      <c r="C308">
+        <v>125.67</v>
+      </c>
+      <c r="D308">
+        <v>0.98</v>
+      </c>
+      <c r="E308">
+        <v>0.7</v>
+      </c>
+      <c r="F308">
+        <v>39.08</v>
+      </c>
+      <c r="G308">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7">
+      <c r="A309" t="s">
+        <v>9</v>
+      </c>
+      <c r="B309">
+        <v>58.07</v>
+      </c>
+      <c r="C309">
+        <v>60.92</v>
+      </c>
+      <c r="D309">
+        <v>0.58</v>
+      </c>
+      <c r="E309">
+        <v>0.5</v>
+      </c>
+      <c r="F309">
+        <v>7.77</v>
+      </c>
+      <c r="G309">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7">
+      <c r="A310" t="s">
+        <v>10</v>
+      </c>
+      <c r="B310">
+        <v>116.21</v>
+      </c>
+      <c r="C310">
+        <v>120.51</v>
+      </c>
+      <c r="D310">
+        <v>1</v>
+      </c>
+      <c r="E310">
+        <v>1</v>
+      </c>
+      <c r="F310">
+        <v>35.48</v>
+      </c>
+      <c r="G310">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7">
+      <c r="A311" t="s">
+        <v>11</v>
+      </c>
+      <c r="B311">
+        <v>182.92</v>
+      </c>
+      <c r="C311">
+        <v>184.04</v>
+      </c>
+      <c r="D311">
+        <v>0.83</v>
+      </c>
+      <c r="E311">
+        <v>0.9</v>
+      </c>
+      <c r="F311">
+        <v>26.76</v>
+      </c>
+      <c r="G311">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7">
+      <c r="A312" t="s">
+        <v>12</v>
+      </c>
+      <c r="B312">
+        <v>52.38</v>
+      </c>
+      <c r="C312">
+        <v>54.86</v>
+      </c>
+      <c r="D312">
+        <v>0.88</v>
+      </c>
+      <c r="E312">
+        <v>0.5</v>
+      </c>
+      <c r="F312">
+        <v>18.66</v>
+      </c>
+      <c r="G312">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7">
+      <c r="A313" t="s">
+        <v>13</v>
+      </c>
+      <c r="B313">
+        <v>56.81</v>
+      </c>
+      <c r="C313">
+        <v>80.43000000000001</v>
+      </c>
+      <c r="D313">
+        <v>0.92</v>
+      </c>
+      <c r="E313">
+        <v>0.7</v>
+      </c>
+      <c r="F313">
+        <v>2.9</v>
+      </c>
+      <c r="G313">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7">
+      <c r="A314" t="s">
+        <v>14</v>
+      </c>
+      <c r="B314">
+        <v>131.41</v>
+      </c>
+      <c r="C314">
+        <v>140.08</v>
+      </c>
+      <c r="D314">
+        <v>1</v>
+      </c>
+      <c r="E314">
+        <v>1</v>
+      </c>
+      <c r="F314">
+        <v>5.13</v>
+      </c>
+      <c r="G314">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7">
+      <c r="A315" t="s">
+        <v>15</v>
+      </c>
+      <c r="B315">
+        <v>77.25</v>
+      </c>
+      <c r="C315">
+        <v>87.23</v>
+      </c>
+      <c r="D315">
+        <v>0.96</v>
+      </c>
+      <c r="E315">
+        <v>0.4</v>
+      </c>
+      <c r="F315">
+        <v>17.01</v>
+      </c>
+      <c r="G315">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7">
+      <c r="A316" t="s">
+        <v>16</v>
+      </c>
+      <c r="B316">
+        <v>160.54</v>
+      </c>
+      <c r="C316">
+        <v>166</v>
+      </c>
+      <c r="D316">
+        <v>0.54</v>
+      </c>
+      <c r="E316">
+        <v>0.4</v>
+      </c>
+      <c r="F316">
+        <v>11.11</v>
+      </c>
+      <c r="G316">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7">
+      <c r="A317" t="s">
+        <v>17</v>
+      </c>
+      <c r="B317">
+        <v>38.77</v>
+      </c>
+      <c r="C317">
+        <v>38.77</v>
+      </c>
+      <c r="D317">
+        <v>0.97</v>
+      </c>
+      <c r="E317">
+        <v>0.6</v>
+      </c>
+      <c r="F317">
+        <v>9.960000000000001</v>
+      </c>
+      <c r="G317">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7">
+      <c r="A318" t="s">
+        <v>18</v>
+      </c>
+      <c r="B318">
+        <v>97.11</v>
+      </c>
+      <c r="C318">
+        <v>110.57</v>
+      </c>
+      <c r="D318">
+        <v>1</v>
+      </c>
+      <c r="E318">
+        <v>1</v>
+      </c>
+      <c r="F318">
+        <v>5.45</v>
+      </c>
+      <c r="G318">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7">
+      <c r="A319" t="s">
+        <v>19</v>
+      </c>
+      <c r="B319">
+        <v>90.45999999999999</v>
+      </c>
+      <c r="C319">
+        <v>106.37</v>
+      </c>
+      <c r="D319">
+        <v>0.95</v>
+      </c>
+      <c r="E319">
+        <v>0.7</v>
+      </c>
+      <c r="F319">
+        <v>12.38</v>
+      </c>
+      <c r="G319">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7">
+      <c r="A320" t="s">
+        <v>20</v>
+      </c>
+      <c r="B320">
+        <v>9.529999999999999</v>
+      </c>
+      <c r="C320">
+        <v>9.67</v>
+      </c>
+      <c r="D320">
+        <v>1</v>
+      </c>
+      <c r="E320">
+        <v>1</v>
+      </c>
+      <c r="F320">
+        <v>13.32</v>
+      </c>
+      <c r="G320">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7">
+      <c r="A321" t="s">
+        <v>21</v>
+      </c>
+      <c r="B321">
+        <v>29.41</v>
+      </c>
+      <c r="C321">
+        <v>33.77</v>
+      </c>
+      <c r="D321">
+        <v>0.66</v>
+      </c>
+      <c r="E321">
+        <v>0.6</v>
+      </c>
+      <c r="F321">
+        <v>24.9</v>
+      </c>
+      <c r="G321">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7">
+      <c r="A322" t="s">
+        <v>22</v>
+      </c>
+      <c r="B322">
+        <v>1.06</v>
+      </c>
+      <c r="C322">
+        <v>1.43</v>
+      </c>
+      <c r="D322">
+        <v>1</v>
+      </c>
+      <c r="E322">
+        <v>1</v>
+      </c>
+      <c r="F322">
+        <v>7.48</v>
+      </c>
+      <c r="G322">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7">
+      <c r="A323" t="s">
+        <v>23</v>
+      </c>
+      <c r="B323" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7">
+      <c r="B324" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C324" s="1"/>
+      <c r="D324" s="1"/>
+      <c r="E324" s="1"/>
+      <c r="F324" s="1"/>
+      <c r="G324" s="1"/>
+    </row>
+    <row r="325" spans="1:7">
+      <c r="B325" t="s">
+        <v>0</v>
+      </c>
+      <c r="C325" t="s">
+        <v>1</v>
+      </c>
+      <c r="D325" t="s">
+        <v>2</v>
+      </c>
+      <c r="E325" t="s">
+        <v>3</v>
+      </c>
+      <c r="F325" t="s">
+        <v>4</v>
+      </c>
+      <c r="G325" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7">
+      <c r="A326" t="s">
+        <v>8</v>
+      </c>
+      <c r="B326">
+        <v>62.95</v>
+      </c>
+      <c r="C326">
+        <v>70.68000000000001</v>
+      </c>
+      <c r="D326">
+        <v>0.95</v>
+      </c>
+      <c r="E326">
+        <v>0.9</v>
+      </c>
+      <c r="F326">
+        <v>40.97</v>
+      </c>
+      <c r="G326">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7">
+      <c r="A327" t="s">
+        <v>9</v>
+      </c>
+      <c r="B327">
+        <v>0</v>
+      </c>
+      <c r="C327">
+        <v>0</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+      <c r="E327">
+        <v>0</v>
+      </c>
+      <c r="F327">
+        <v>0</v>
+      </c>
+      <c r="G327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7">
+      <c r="A328" t="s">
+        <v>10</v>
+      </c>
+      <c r="B328">
+        <v>0</v>
+      </c>
+      <c r="C328">
+        <v>0</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+      <c r="E328">
+        <v>0</v>
+      </c>
+      <c r="F328">
+        <v>0</v>
+      </c>
+      <c r="G328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7">
+      <c r="A329" t="s">
+        <v>11</v>
+      </c>
+      <c r="B329">
+        <v>126.22</v>
+      </c>
+      <c r="C329">
+        <v>137.44</v>
+      </c>
+      <c r="D329">
+        <v>0.8</v>
+      </c>
+      <c r="E329">
+        <v>0.7</v>
+      </c>
+      <c r="F329">
+        <v>22.01</v>
+      </c>
+      <c r="G329">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7">
+      <c r="A330" t="s">
+        <v>12</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+      <c r="C330">
+        <v>0</v>
+      </c>
+      <c r="D330">
+        <v>0</v>
+      </c>
+      <c r="E330">
+        <v>0</v>
+      </c>
+      <c r="F330">
+        <v>0</v>
+      </c>
+      <c r="G330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7">
+      <c r="A331" t="s">
+        <v>13</v>
+      </c>
+      <c r="B331">
+        <v>46.38</v>
+      </c>
+      <c r="C331">
+        <v>62.5</v>
+      </c>
+      <c r="D331">
+        <v>0.98</v>
+      </c>
+      <c r="E331">
+        <v>0.7</v>
+      </c>
+      <c r="F331">
+        <v>5.09</v>
+      </c>
+      <c r="G331">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7">
+      <c r="A332" t="s">
+        <v>14</v>
+      </c>
+      <c r="B332">
+        <v>112.68</v>
+      </c>
+      <c r="C332">
+        <v>118.02</v>
+      </c>
+      <c r="D332">
+        <v>1</v>
+      </c>
+      <c r="E332">
+        <v>1</v>
+      </c>
+      <c r="F332">
+        <v>2.86</v>
+      </c>
+      <c r="G332">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7">
+      <c r="A333" t="s">
+        <v>15</v>
+      </c>
+      <c r="B333">
+        <v>0</v>
+      </c>
+      <c r="C333">
+        <v>0</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+      <c r="E333">
+        <v>0</v>
+      </c>
+      <c r="F333">
+        <v>0</v>
+      </c>
+      <c r="G333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7">
+      <c r="A334" t="s">
+        <v>16</v>
+      </c>
+      <c r="B334">
+        <v>87.34999999999999</v>
+      </c>
+      <c r="C334">
+        <v>119.32</v>
+      </c>
+      <c r="D334">
+        <v>0.5</v>
+      </c>
+      <c r="E334">
+        <v>0.25</v>
+      </c>
+      <c r="F334">
+        <v>31.08</v>
+      </c>
+      <c r="G334">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7">
+      <c r="A335" t="s">
+        <v>17</v>
+      </c>
+      <c r="B335">
+        <v>0</v>
+      </c>
+      <c r="C335">
+        <v>0</v>
+      </c>
+      <c r="D335">
+        <v>0</v>
+      </c>
+      <c r="E335">
+        <v>0</v>
+      </c>
+      <c r="F335">
+        <v>0</v>
+      </c>
+      <c r="G335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7">
+      <c r="A336" t="s">
+        <v>18</v>
+      </c>
+      <c r="B336">
+        <v>70.19</v>
+      </c>
+      <c r="C336">
+        <v>76.22</v>
+      </c>
+      <c r="D336">
+        <v>1</v>
+      </c>
+      <c r="E336">
+        <v>1</v>
+      </c>
+      <c r="F336">
+        <v>6.68</v>
+      </c>
+      <c r="G336">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7">
+      <c r="A337" t="s">
+        <v>19</v>
+      </c>
+      <c r="B337">
+        <v>92.09</v>
+      </c>
+      <c r="C337">
+        <v>93.33</v>
+      </c>
+      <c r="D337">
+        <v>1</v>
+      </c>
+      <c r="E337">
+        <v>1</v>
+      </c>
+      <c r="F337">
+        <v>9.26</v>
+      </c>
+      <c r="G337">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7">
+      <c r="A338" t="s">
+        <v>20</v>
+      </c>
+      <c r="B338">
+        <v>9.529999999999999</v>
+      </c>
+      <c r="C338">
+        <v>9.67</v>
+      </c>
+      <c r="D338">
+        <v>1</v>
+      </c>
+      <c r="E338">
+        <v>1</v>
+      </c>
+      <c r="F338">
+        <v>12.75</v>
+      </c>
+      <c r="G338">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7">
+      <c r="A339" t="s">
+        <v>21</v>
+      </c>
+      <c r="B339">
+        <v>0</v>
+      </c>
+      <c r="C339">
+        <v>0</v>
+      </c>
+      <c r="D339">
+        <v>0</v>
+      </c>
+      <c r="E339">
+        <v>0</v>
+      </c>
+      <c r="F339">
+        <v>0</v>
+      </c>
+      <c r="G339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7">
+      <c r="A340" t="s">
+        <v>22</v>
+      </c>
+      <c r="B340">
+        <v>0</v>
+      </c>
+      <c r="C340">
+        <v>0</v>
+      </c>
+      <c r="D340">
+        <v>0</v>
+      </c>
+      <c r="E340">
+        <v>0</v>
+      </c>
+      <c r="F340">
+        <v>0</v>
+      </c>
+      <c r="G340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7">
+      <c r="A341" t="s">
+        <v>23</v>
+      </c>
+      <c r="B341" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7">
+      <c r="B343" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C343" s="1"/>
+      <c r="D343" s="1"/>
+      <c r="E343" s="1"/>
+      <c r="F343" s="1"/>
+      <c r="G343" s="1"/>
+    </row>
+    <row r="344" spans="1:7">
+      <c r="B344" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C344" s="1"/>
+      <c r="D344" s="1"/>
+      <c r="E344" s="1"/>
+      <c r="F344" s="1"/>
+      <c r="G344" s="1"/>
+    </row>
+    <row r="345" spans="1:7">
+      <c r="B345" t="s">
+        <v>0</v>
+      </c>
+      <c r="C345" t="s">
+        <v>1</v>
+      </c>
+      <c r="D345" t="s">
+        <v>2</v>
+      </c>
+      <c r="E345" t="s">
+        <v>3</v>
+      </c>
+      <c r="F345" t="s">
+        <v>4</v>
+      </c>
+      <c r="G345" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7">
+      <c r="A346" t="s">
+        <v>8</v>
+      </c>
+      <c r="B346">
+        <v>114.36</v>
+      </c>
+      <c r="C346">
+        <v>125.67</v>
+      </c>
+      <c r="D346">
+        <v>0.98</v>
+      </c>
+      <c r="E346">
+        <v>0.6</v>
+      </c>
+      <c r="F346">
+        <v>33.6</v>
+      </c>
+      <c r="G346">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7">
+      <c r="A347" t="s">
+        <v>9</v>
+      </c>
+      <c r="B347">
+        <v>58.07</v>
+      </c>
+      <c r="C347">
+        <v>60.92</v>
+      </c>
+      <c r="D347">
+        <v>0.97</v>
+      </c>
+      <c r="E347">
+        <v>0.8</v>
+      </c>
+      <c r="F347">
+        <v>5.45</v>
+      </c>
+      <c r="G347">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7">
+      <c r="A348" t="s">
+        <v>10</v>
+      </c>
+      <c r="B348">
+        <v>116.21</v>
+      </c>
+      <c r="C348">
+        <v>120.51</v>
+      </c>
+      <c r="D348">
+        <v>1</v>
+      </c>
+      <c r="E348">
+        <v>1</v>
+      </c>
+      <c r="F348">
+        <v>26.11</v>
+      </c>
+      <c r="G348">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7">
+      <c r="A349" t="s">
+        <v>11</v>
+      </c>
+      <c r="B349">
+        <v>182.92</v>
+      </c>
+      <c r="C349">
+        <v>184.04</v>
+      </c>
+      <c r="D349">
+        <v>1</v>
+      </c>
+      <c r="E349">
+        <v>1</v>
+      </c>
+      <c r="F349">
+        <v>24.65</v>
+      </c>
+      <c r="G349">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7">
+      <c r="A350" t="s">
+        <v>12</v>
+      </c>
+      <c r="B350">
+        <v>52.38</v>
+      </c>
+      <c r="C350">
+        <v>54.86</v>
+      </c>
+      <c r="D350">
+        <v>0.99</v>
+      </c>
+      <c r="E350">
+        <v>0.9</v>
+      </c>
+      <c r="F350">
+        <v>12.71</v>
+      </c>
+      <c r="G350">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7">
+      <c r="A351" t="s">
+        <v>13</v>
+      </c>
+      <c r="B351">
+        <v>56.81</v>
+      </c>
+      <c r="C351">
+        <v>80.43000000000001</v>
+      </c>
+      <c r="D351">
+        <v>0.97</v>
+      </c>
+      <c r="E351">
+        <v>0.8</v>
+      </c>
+      <c r="F351">
+        <v>4.26</v>
+      </c>
+      <c r="G351">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7">
+      <c r="A352" t="s">
+        <v>14</v>
+      </c>
+      <c r="B352">
+        <v>131.41</v>
+      </c>
+      <c r="C352">
+        <v>140.08</v>
+      </c>
+      <c r="D352">
+        <v>1</v>
+      </c>
+      <c r="E352">
+        <v>1</v>
+      </c>
+      <c r="F352">
+        <v>4.88</v>
+      </c>
+      <c r="G352">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7">
+      <c r="A353" t="s">
+        <v>15</v>
+      </c>
+      <c r="B353">
+        <v>77.25</v>
+      </c>
+      <c r="C353">
+        <v>87.23</v>
+      </c>
+      <c r="D353">
+        <v>1</v>
+      </c>
+      <c r="E353">
+        <v>1</v>
+      </c>
+      <c r="F353">
+        <v>10.59</v>
+      </c>
+      <c r="G353">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7">
+      <c r="A354" t="s">
+        <v>16</v>
+      </c>
+      <c r="B354">
+        <v>160.54</v>
+      </c>
+      <c r="C354">
+        <v>166</v>
+      </c>
+      <c r="D354">
+        <v>0.91</v>
+      </c>
+      <c r="E354">
+        <v>0.8</v>
+      </c>
+      <c r="F354">
+        <v>10.67</v>
+      </c>
+      <c r="G354">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7">
+      <c r="A355" t="s">
+        <v>17</v>
+      </c>
+      <c r="B355">
+        <v>38.77</v>
+      </c>
+      <c r="C355">
+        <v>38.77</v>
+      </c>
+      <c r="D355">
+        <v>1</v>
+      </c>
+      <c r="E355">
+        <v>1</v>
+      </c>
+      <c r="F355">
+        <v>4.63</v>
+      </c>
+      <c r="G355">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7">
+      <c r="A356" t="s">
+        <v>18</v>
+      </c>
+      <c r="B356">
+        <v>97.11</v>
+      </c>
+      <c r="C356">
+        <v>110.57</v>
+      </c>
+      <c r="D356">
+        <v>1</v>
+      </c>
+      <c r="E356">
+        <v>1</v>
+      </c>
+      <c r="F356">
+        <v>5.83</v>
+      </c>
+      <c r="G356">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7">
+      <c r="A357" t="s">
+        <v>19</v>
+      </c>
+      <c r="B357">
+        <v>90.45999999999999</v>
+      </c>
+      <c r="C357">
+        <v>106.37</v>
+      </c>
+      <c r="D357">
+        <v>1</v>
+      </c>
+      <c r="E357">
+        <v>1</v>
+      </c>
+      <c r="F357">
+        <v>11.06</v>
+      </c>
+      <c r="G357">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7">
+      <c r="A358" t="s">
+        <v>20</v>
+      </c>
+      <c r="B358">
+        <v>9.529999999999999</v>
+      </c>
+      <c r="C358">
+        <v>9.67</v>
+      </c>
+      <c r="D358">
+        <v>1</v>
+      </c>
+      <c r="E358">
+        <v>1</v>
+      </c>
+      <c r="F358">
+        <v>13.01</v>
+      </c>
+      <c r="G358">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7">
+      <c r="A359" t="s">
+        <v>21</v>
+      </c>
+      <c r="B359">
+        <v>29.41</v>
+      </c>
+      <c r="C359">
+        <v>33.77</v>
+      </c>
+      <c r="D359">
+        <v>1</v>
+      </c>
+      <c r="E359">
+        <v>1</v>
+      </c>
+      <c r="F359">
+        <v>30.54</v>
+      </c>
+      <c r="G359">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7">
+      <c r="A360" t="s">
+        <v>22</v>
+      </c>
+      <c r="B360">
+        <v>1.06</v>
+      </c>
+      <c r="C360">
+        <v>1.43</v>
+      </c>
+      <c r="D360">
+        <v>1</v>
+      </c>
+      <c r="E360">
+        <v>1</v>
+      </c>
+      <c r="F360">
+        <v>8.460000000000001</v>
+      </c>
+      <c r="G360">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7">
+      <c r="A361" t="s">
+        <v>23</v>
+      </c>
+      <c r="B361" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7">
+      <c r="B362" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C362" s="1"/>
+      <c r="D362" s="1"/>
+      <c r="E362" s="1"/>
+      <c r="F362" s="1"/>
+      <c r="G362" s="1"/>
+    </row>
+    <row r="363" spans="1:7">
+      <c r="B363" t="s">
+        <v>0</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1</v>
+      </c>
+      <c r="D363" t="s">
+        <v>2</v>
+      </c>
+      <c r="E363" t="s">
+        <v>3</v>
+      </c>
+      <c r="F363" t="s">
+        <v>4</v>
+      </c>
+      <c r="G363" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7">
+      <c r="A364" t="s">
+        <v>8</v>
+      </c>
+      <c r="B364">
+        <v>62.95</v>
+      </c>
+      <c r="C364">
+        <v>70.68000000000001</v>
+      </c>
+      <c r="D364">
+        <v>0.95</v>
+      </c>
+      <c r="E364">
+        <v>0.9</v>
+      </c>
+      <c r="F364">
+        <v>36.86</v>
+      </c>
+      <c r="G364">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7">
+      <c r="A365" t="s">
+        <v>9</v>
+      </c>
+      <c r="B365">
+        <v>0</v>
+      </c>
+      <c r="C365">
+        <v>0</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365">
+        <v>0</v>
+      </c>
+      <c r="F365">
+        <v>0</v>
+      </c>
+      <c r="G365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7">
+      <c r="A366" t="s">
+        <v>10</v>
+      </c>
+      <c r="B366">
+        <v>0</v>
+      </c>
+      <c r="C366">
+        <v>0</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366">
+        <v>0</v>
+      </c>
+      <c r="F366">
+        <v>0</v>
+      </c>
+      <c r="G366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7">
+      <c r="A367" t="s">
+        <v>11</v>
+      </c>
+      <c r="B367">
+        <v>126.22</v>
+      </c>
+      <c r="C367">
+        <v>137.44</v>
+      </c>
+      <c r="D367">
+        <v>1</v>
+      </c>
+      <c r="E367">
+        <v>1</v>
+      </c>
+      <c r="F367">
+        <v>26.88</v>
+      </c>
+      <c r="G367">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7">
+      <c r="A368" t="s">
+        <v>12</v>
+      </c>
+      <c r="B368">
+        <v>0</v>
+      </c>
+      <c r="C368">
+        <v>0</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+      <c r="E368">
+        <v>0</v>
+      </c>
+      <c r="F368">
+        <v>0</v>
+      </c>
+      <c r="G368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7">
+      <c r="A369" t="s">
+        <v>13</v>
+      </c>
+      <c r="B369">
+        <v>46.38</v>
+      </c>
+      <c r="C369">
+        <v>62.5</v>
+      </c>
+      <c r="D369">
+        <v>1</v>
+      </c>
+      <c r="E369">
+        <v>0.8</v>
+      </c>
+      <c r="F369">
+        <v>2.86</v>
+      </c>
+      <c r="G369">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7">
+      <c r="A370" t="s">
+        <v>14</v>
+      </c>
+      <c r="B370">
+        <v>112.68</v>
+      </c>
+      <c r="C370">
+        <v>118.02</v>
+      </c>
+      <c r="D370">
+        <v>1</v>
+      </c>
+      <c r="E370">
+        <v>1</v>
+      </c>
+      <c r="F370">
+        <v>3.77</v>
+      </c>
+      <c r="G370">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7">
+      <c r="A371" t="s">
+        <v>15</v>
+      </c>
+      <c r="B371">
+        <v>22.66</v>
+      </c>
+      <c r="C371">
+        <v>44.04</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+      <c r="E371">
+        <v>0</v>
+      </c>
+      <c r="F371">
+        <v>8.99</v>
+      </c>
+      <c r="G371">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7">
+      <c r="A372" t="s">
+        <v>16</v>
+      </c>
+      <c r="B372">
+        <v>87.34999999999999</v>
+      </c>
+      <c r="C372">
+        <v>119.32</v>
+      </c>
+      <c r="D372">
+        <v>0.5</v>
+      </c>
+      <c r="E372">
+        <v>0.25</v>
+      </c>
+      <c r="F372">
+        <v>12.63</v>
+      </c>
+      <c r="G372">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7">
+      <c r="A373" t="s">
+        <v>17</v>
+      </c>
+      <c r="B373">
+        <v>0</v>
+      </c>
+      <c r="C373">
+        <v>0</v>
+      </c>
+      <c r="D373">
+        <v>0</v>
+      </c>
+      <c r="E373">
+        <v>0</v>
+      </c>
+      <c r="F373">
+        <v>0</v>
+      </c>
+      <c r="G373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7">
+      <c r="A374" t="s">
+        <v>18</v>
+      </c>
+      <c r="B374">
+        <v>70.19</v>
+      </c>
+      <c r="C374">
+        <v>76.22</v>
+      </c>
+      <c r="D374">
+        <v>1</v>
+      </c>
+      <c r="E374">
+        <v>1</v>
+      </c>
+      <c r="F374">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="G374">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7">
+      <c r="A375" t="s">
+        <v>19</v>
+      </c>
+      <c r="B375">
+        <v>92.09</v>
+      </c>
+      <c r="C375">
+        <v>93.33</v>
+      </c>
+      <c r="D375">
+        <v>1</v>
+      </c>
+      <c r="E375">
+        <v>0.8</v>
+      </c>
+      <c r="F375">
+        <v>11.97</v>
+      </c>
+      <c r="G375">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7">
+      <c r="A376" t="s">
+        <v>20</v>
+      </c>
+      <c r="B376">
+        <v>9.529999999999999</v>
+      </c>
+      <c r="C376">
+        <v>9.67</v>
+      </c>
+      <c r="D376">
+        <v>1</v>
+      </c>
+      <c r="E376">
+        <v>1</v>
+      </c>
+      <c r="F376">
+        <v>12.2</v>
+      </c>
+      <c r="G376">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7">
+      <c r="A377" t="s">
+        <v>21</v>
+      </c>
+      <c r="B377">
+        <v>29.42</v>
+      </c>
+      <c r="C377">
+        <v>37.12</v>
+      </c>
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377">
+        <v>0</v>
+      </c>
+      <c r="F377">
+        <v>22.5</v>
+      </c>
+      <c r="G377">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7">
+      <c r="A378" t="s">
+        <v>22</v>
+      </c>
+      <c r="B378">
+        <v>0</v>
+      </c>
+      <c r="C378">
+        <v>0</v>
+      </c>
+      <c r="D378">
+        <v>0</v>
+      </c>
+      <c r="E378">
+        <v>0</v>
+      </c>
+      <c r="F378">
+        <v>0</v>
+      </c>
+      <c r="G378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7">
+      <c r="A379" t="s">
+        <v>23</v>
+      </c>
+      <c r="B379" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B20:G20"/>
@@ -6737,6 +8307,12 @@
     <mergeCell ref="B267:G267"/>
     <mergeCell ref="B268:G268"/>
     <mergeCell ref="B286:G286"/>
+    <mergeCell ref="B305:G305"/>
+    <mergeCell ref="B306:G306"/>
+    <mergeCell ref="B324:G324"/>
+    <mergeCell ref="B343:G343"/>
+    <mergeCell ref="B344:G344"/>
+    <mergeCell ref="B362:G362"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>